<commit_message>
17.11.22 - even worse program
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoC\Clash_Bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\Clash_Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EAD6B50-2C0B-411A-9472-25F9FA29090E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713A5526-BFCC-4FB1-8099-9DA2C4D49D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Angriffe" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Time</t>
   </si>
@@ -377,19 +377,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" style="4" customWidth="1"/>
     <col min="2" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -409,7 +409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>44882.052322847223</v>
       </c>
@@ -429,9 +429,9 @@
         <v>5872</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>44882.057733025598</v>
+        <v>44882.057733020833</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -447,6 +447,46 @@
       </c>
       <c r="F3">
         <v>7715</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>44882.381963749998</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>515340</v>
+      </c>
+      <c r="E4">
+        <v>793494</v>
+      </c>
+      <c r="F4">
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>44882.472736634998</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>193202</v>
+      </c>
+      <c r="E5">
+        <v>57778</v>
+      </c>
+      <c r="F5">
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>